<commit_message>
XLL_ENUM now working Fix OPER constructor from int to create num. Bug fix in newton 1-d root finding. Memoize Bell
</commit_message>
<xml_diff>
--- a/test/njr.xlsx
+++ b/test/njr.xlsx
@@ -88,7 +88,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -180,7 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -465,7 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -498,11 +500,11 @@
       </c>
       <c r="H4" s="6">
         <f>_xll.NJR.CDF(x, H11:H26)</f>
-        <v>0.50000663911759502</v>
+        <v>0.96542731830315209</v>
       </c>
       <c r="L4" s="2">
         <f>F4-H4</f>
-        <v>-9.9363995920143111E-9</v>
+        <v>-0.46542068912195667</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.55000000000000004">
@@ -577,7 +579,7 @@
       </c>
       <c r="K9">
         <f>I5  - I6*SUM(K11:K40)</f>
-        <v>0.50000663911759502</v>
+        <v>0.96542731830315209</v>
       </c>
       <c r="L9" s="8">
         <f>H4-K9</f>
@@ -599,7 +601,7 @@
         <v>0.5039893563146316</v>
       </c>
       <c r="F10">
-        <f>EXP(-lambda)*E10*D10/C10</f>
+        <f t="shared" ref="F10:F40" si="0">EXP(-lambda)*E10*D10/C10</f>
         <v>0.45602842788533648</v>
       </c>
       <c r="O10" t="s">
@@ -618,7 +620,7 @@
         <v>1</v>
       </c>
       <c r="D11">
-        <f>lambda^B11</f>
+        <f t="shared" ref="D11:D40" si="1">lambda^B11</f>
         <v>0.1</v>
       </c>
       <c r="E11">
@@ -626,7 +628,7 @@
         <v>0.46414360741482791</v>
       </c>
       <c r="F11">
-        <f>EXP(-lambda)*E11*D11/C11</f>
+        <f t="shared" si="0"/>
         <v>4.199745033311289E-2</v>
       </c>
       <c r="H11">
@@ -634,7 +636,7 @@
       </c>
       <c r="I11">
         <f>_xll.BELL(H11)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="J11">
         <f>_xll.HERMITE(B10, x)</f>
@@ -642,7 +644,7 @@
       </c>
       <c r="K11">
         <f>I11*J11/C11</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="O11" s="7">
         <v>1</v>
@@ -661,7 +663,7 @@
         <v>2</v>
       </c>
       <c r="D12">
-        <f>lambda^B12</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="E12">
@@ -669,7 +671,7 @@
         <v>0.42465456526520451</v>
       </c>
       <c r="F12">
-        <f>EXP(-lambda)*E12*D12/C12</f>
+        <f t="shared" si="0"/>
         <v>1.921216701958753E-3</v>
       </c>
       <c r="H12">
@@ -677,14 +679,14 @@
       </c>
       <c r="I12">
         <f>_xll.BELL($H$11:H12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <f>_xll.HERMITE(B11, x)</f>
         <v>0</v>
       </c>
       <c r="K12">
-        <f t="shared" ref="K12:K40" si="0">I12*J12/C12</f>
+        <f t="shared" ref="K12:K40" si="2">I12*J12/C12</f>
         <v>0</v>
       </c>
       <c r="M12" t="s">
@@ -698,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" ref="P12:P15" si="1">J12-O12</f>
+        <f t="shared" ref="P12:P15" si="3">J12-O12</f>
         <v>0</v>
       </c>
     </row>
@@ -707,11 +709,11 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C40" si="2">B13*C12</f>
+        <f t="shared" ref="C13:C40" si="4">B13*C12</f>
         <v>6</v>
       </c>
       <c r="D13">
-        <f>lambda^B13</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000002E-3</v>
       </c>
       <c r="E13">
@@ -719,24 +721,24 @@
         <v>0.38590811880112263</v>
       </c>
       <c r="F13">
-        <f>EXP(-lambda)*E13*D13/C13</f>
+        <f t="shared" si="0"/>
         <v>5.8197350969187027E-5</v>
       </c>
       <c r="H13">
-        <f>const^B13*lambda</f>
+        <f t="shared" ref="H13:H40" si="5">const^B13*lambda</f>
         <v>1.0000000000000003E-4</v>
       </c>
       <c r="I13">
         <f>_xll.BELL($H$11:H13)</f>
-        <v>1.0000000000000003E-4</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <f>_xll.HERMITE(B12, x)</f>
         <v>-1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
-        <v>-1.6666666666666671E-5</v>
+        <f t="shared" si="2"/>
+        <v>-0.16666666666666666</v>
       </c>
       <c r="M13" s="7">
         <f>H13</f>
@@ -744,14 +746,14 @@
       </c>
       <c r="N13" s="3">
         <f>I13-M13</f>
-        <v>0</v>
+        <v>0.99990000000000001</v>
       </c>
       <c r="O13" s="7">
         <f>x^2-1</f>
         <v>-1</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -760,11 +762,11 @@
         <v>4</v>
       </c>
       <c r="C14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="D14">
-        <f>lambda^B14</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000005E-4</v>
       </c>
       <c r="E14">
@@ -772,23 +774,23 @@
         <v>0.34826827346401767</v>
       </c>
       <c r="F14">
-        <f>EXP(-lambda)*E14*D14/C14</f>
+        <f t="shared" si="0"/>
         <v>1.3130256889375975E-6</v>
       </c>
       <c r="H14">
-        <f>const^B14*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000006E-5</v>
       </c>
       <c r="I14">
         <f>_xll.BELL($H$11:H14)</f>
-        <v>1.0000000000000006E-5</v>
+        <v>-2.9000000000000006E-4</v>
       </c>
       <c r="J14">
         <f>_xll.HERMITE(B13, x)</f>
         <v>0</v>
       </c>
       <c r="K14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M14" s="7">
@@ -796,15 +798,15 @@
         <v>1.0000000000000006E-5</v>
       </c>
       <c r="N14" s="4">
-        <f t="shared" ref="N14:N17" si="3">I14-M14</f>
-        <v>0</v>
+        <f t="shared" ref="N14:N17" si="6">I14-M14</f>
+        <v>-3.0000000000000008E-4</v>
       </c>
       <c r="O14" s="7">
         <f>x^3-3*x</f>
         <v>0</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -813,11 +815,11 @@
         <v>5</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="D15">
-        <f>lambda^B15</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000006E-5</v>
       </c>
       <c r="E15">
@@ -825,39 +827,39 @@
         <v>0.31206694941739055</v>
       </c>
       <c r="F15">
-        <f>EXP(-lambda)*E15*D15/C15</f>
+        <f t="shared" si="0"/>
         <v>2.3530821063765854E-8</v>
       </c>
       <c r="H15">
-        <f>const^B15*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000006E-6</v>
       </c>
       <c r="I15">
         <f>_xll.BELL($H$11:H15)</f>
-        <v>1.0000000000000006E-6</v>
+        <v>5.6100000000000019E-4</v>
       </c>
       <c r="J15">
         <f>_xll.HERMITE(B14, x)</f>
         <v>3</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000015E-8</v>
+        <f t="shared" si="2"/>
+        <v>1.4025000000000004E-5</v>
       </c>
       <c r="M15" s="7">
         <f>H15</f>
         <v>1.0000000000000006E-6</v>
       </c>
       <c r="N15" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>5.6000000000000017E-4</v>
       </c>
       <c r="O15" s="7">
         <f>x^4-6*x^2+3</f>
         <v>3</v>
       </c>
       <c r="P15" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -866,11 +868,11 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>720</v>
       </c>
       <c r="D16">
-        <f>lambda^B16</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000006E-6</v>
       </c>
       <c r="E16">
@@ -878,23 +880,23 @@
         <v>0.27759532475346488</v>
       </c>
       <c r="F16">
-        <f>EXP(-lambda)*E16*D16/C16</f>
+        <f t="shared" si="0"/>
         <v>3.488592179288597E-10</v>
       </c>
       <c r="H16">
-        <f>const^B16*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000006E-7</v>
       </c>
       <c r="I16">
         <f>_xll.BELL($H$11:H16)</f>
-        <v>2.0000000000000012E-7</v>
+        <v>1.0951000000000003E-3</v>
       </c>
       <c r="J16">
         <f>_xll.HERMITE(B15, x)</f>
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M16" s="7">
@@ -902,8 +904,8 @@
         <v>2.0000000000000015E-7</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1.0949000000000004E-3</v>
       </c>
     </row>
     <row r="17" spans="2:14" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -911,11 +913,11 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5040</v>
       </c>
       <c r="D17">
-        <f>lambda^B17</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000007E-7</v>
       </c>
       <c r="E17">
@@ -923,32 +925,32 @@
         <v>0.24509709367430949</v>
       </c>
       <c r="F17">
-        <f>EXP(-lambda)*E17*D17/C17</f>
+        <f t="shared" si="0"/>
         <v>4.4002583612773818E-12</v>
       </c>
       <c r="H17">
-        <f>const^B17*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000008E-8</v>
       </c>
       <c r="I17">
         <f>_xll.BELL($H$11:H17)</f>
-        <v>4.5000000000000046E-8</v>
+        <v>2.1397500000000015E-4</v>
       </c>
       <c r="J17">
         <f>_xll.HERMITE(B16, x)</f>
         <v>-15</v>
       </c>
       <c r="K17">
-        <f t="shared" si="0"/>
-        <v>-1.3392857142857159E-10</v>
+        <f t="shared" si="2"/>
+        <v>-6.368303571428576E-7</v>
       </c>
       <c r="M17" s="7">
         <f>H17+35*H13*H14</f>
         <v>4.5000000000000039E-8</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>2.1393000000000014E-4</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -956,11 +958,11 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40320</v>
       </c>
       <c r="D18">
-        <f>lambda^B18</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000008E-8</v>
       </c>
       <c r="E18">
@@ -968,23 +970,23 @@
         <v>0.21476388416363706</v>
       </c>
       <c r="F18">
-        <f>EXP(-lambda)*E18*D18/C18</f>
+        <f t="shared" si="0"/>
         <v>4.8196031357638744E-14</v>
       </c>
       <c r="H18">
-        <f>const^B18*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000009E-9</v>
       </c>
       <c r="I18">
         <f>_xll.BELL($H$11:H18)</f>
-        <v>1.0100000000000009E-8</v>
+        <v>3.8107600000000035E-5</v>
       </c>
       <c r="J18">
         <f>_xll.HERMITE(B17, x)</f>
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -993,11 +995,11 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>362880</v>
       </c>
       <c r="D19">
-        <f>lambda^B19</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000009E-9</v>
       </c>
       <c r="E19">
@@ -1005,24 +1007,24 @@
         <v>0.18673294303717264</v>
       </c>
       <c r="F19">
-        <f>EXP(-lambda)*E19*D19/C19</f>
+        <f t="shared" si="0"/>
         <v>4.6561660615082488E-16</v>
       </c>
       <c r="H19">
-        <f>const^B19*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000009E-10</v>
       </c>
       <c r="I19">
         <f>_xll.BELL($H$11:H19)</f>
-        <v>2.4800000000000026E-9</v>
+        <v>9.2322400000000056E-6</v>
       </c>
       <c r="J19">
         <f>_xll.HERMITE(B18, x)</f>
         <v>105</v>
       </c>
       <c r="K19">
-        <f t="shared" si="0"/>
-        <v>7.1759259259259344E-13</v>
+        <f t="shared" si="2"/>
+        <v>2.6713657407407424E-9</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1030,11 +1032,11 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3628800</v>
       </c>
       <c r="D20">
-        <f>lambda^B20</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000011E-10</v>
       </c>
       <c r="E20">
@@ -1042,23 +1044,23 @@
         <v>0.16108705951083091</v>
       </c>
       <c r="F20">
-        <f>EXP(-lambda)*E20*D20/C20</f>
+        <f t="shared" si="0"/>
         <v>4.0166886851517125E-18</v>
       </c>
       <c r="H20">
-        <f>const^B20*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000011E-11</v>
       </c>
       <c r="I20">
         <f>_xll.BELL($H$11:H20)</f>
-        <v>6.7600000000000087E-10</v>
+        <v>2.6323360000000025E-6</v>
       </c>
       <c r="J20">
         <f>_xll.HERMITE(B19, x)</f>
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1067,11 +1069,11 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39916800</v>
       </c>
       <c r="D21">
-        <f>lambda^B21</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000011E-11</v>
       </c>
       <c r="E21">
@@ -1079,24 +1081,24 @@
         <v>0.1378565720320355</v>
       </c>
       <c r="F21">
-        <f>EXP(-lambda)*E21*D21/C21</f>
+        <f t="shared" si="0"/>
         <v>3.1249445019830097E-20</v>
       </c>
       <c r="H21">
-        <f>const^B21*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000012E-12</v>
       </c>
       <c r="I21">
         <f>_xll.BELL($H$11:H21)</f>
-        <v>2.0065000000000026E-10</v>
+        <v>7.9615440000000102E-7</v>
       </c>
       <c r="J21">
         <f>_xll.HERMITE(B20, x)</f>
         <v>-945</v>
       </c>
       <c r="K21">
-        <f t="shared" si="0"/>
-        <v>-4.7502367424242487E-15</v>
+        <f t="shared" si="2"/>
+        <v>-1.8848352272727296E-11</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1104,11 +1106,11 @@
         <v>12</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>479001600</v>
       </c>
       <c r="D22">
-        <f>lambda^B22</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000014E-12</v>
       </c>
       <c r="E22">
@@ -1116,23 +1118,23 @@
         <v>0.11702319602310873</v>
       </c>
       <c r="F22">
-        <f>EXP(-lambda)*E22*D22/C22</f>
+        <f t="shared" si="0"/>
         <v>2.2105764686352996E-22</v>
       </c>
       <c r="H22">
-        <f>const^B22*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000014E-13</v>
       </c>
       <c r="I22">
         <f>_xll.BELL($H$11:H22)</f>
-        <v>6.4065000000000104E-11</v>
+        <v>2.5439545000000028E-7</v>
       </c>
       <c r="J22">
         <f>_xll.HERMITE(B21, x)</f>
         <v>0</v>
       </c>
       <c r="K22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1141,11 +1143,11 @@
         <v>13</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6227020800</v>
       </c>
       <c r="D23">
-        <f>lambda^B23</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000014E-13</v>
       </c>
       <c r="E23">
@@ -1153,24 +1155,24 @@
         <v>9.8525329049747812E-2</v>
       </c>
       <c r="F23">
-        <f>EXP(-lambda)*E23*D23/C23</f>
+        <f t="shared" si="0"/>
         <v>1.431654192459374E-24</v>
       </c>
       <c r="H23">
-        <f>const^B23*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000014E-14</v>
       </c>
       <c r="I23">
         <f>_xll.BELL($H$11:H23)</f>
-        <v>2.1846100000000034E-11</v>
+        <v>8.6307918600000091E-8</v>
       </c>
       <c r="J23">
         <f>_xll.HERMITE(B22, x)</f>
         <v>10395</v>
       </c>
       <c r="K23">
-        <f t="shared" si="0"/>
-        <v>3.6468516292735097E-17</v>
+        <f t="shared" si="2"/>
+        <v>1.4407705428685912E-13</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1178,11 +1180,11 @@
         <v>14</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>87178291200</v>
       </c>
       <c r="D24">
-        <f>lambda^B24</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000014E-14</v>
       </c>
       <c r="E24">
@@ -1190,23 +1192,23 @@
         <v>8.2264438677668916E-2</v>
       </c>
       <c r="F24">
-        <f>EXP(-lambda)*E24*D24/C24</f>
+        <f t="shared" si="0"/>
         <v>8.5383575732761742E-27</v>
       </c>
       <c r="H24">
-        <f>const^B24*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000015E-15</v>
       </c>
       <c r="I24">
         <f>_xll.BELL($H$11:H24)</f>
-        <v>7.9167000000000129E-12</v>
+        <v>3.1158785800000036E-8</v>
       </c>
       <c r="J24">
         <f>_xll.HERMITE(B23, x)</f>
         <v>0</v>
       </c>
       <c r="K24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1215,11 +1217,11 @@
         <v>15</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1307674368000</v>
       </c>
       <c r="D25">
-        <f>lambda^B25</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000017E-15</v>
       </c>
       <c r="E25">
@@ -1227,24 +1229,24 @@
         <v>6.8112117966725561E-2</v>
       </c>
       <c r="F25">
-        <f>EXP(-lambda)*E25*D25/C25</f>
+        <f t="shared" si="0"/>
         <v>4.712977058060126E-29</v>
       </c>
       <c r="H25">
-        <f>const^B25*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000017E-16</v>
       </c>
       <c r="I25">
         <f>_xll.BELL($H$11:H25)</f>
-        <v>3.038102500000006E-12</v>
+        <v>1.1952092383000019E-8</v>
       </c>
       <c r="J25">
         <f>_xll.HERMITE(B24, x)</f>
         <v>-135135</v>
       </c>
       <c r="K25">
-        <f t="shared" si="0"/>
-        <v>-3.1395735160383663E-19</v>
+        <f t="shared" si="2"/>
+        <v>-1.2351285944733816E-15</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1252,11 +1254,11 @@
         <v>16</v>
       </c>
       <c r="C26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20922789888000</v>
       </c>
       <c r="D26">
-        <f>lambda^B26</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000017E-16</v>
       </c>
       <c r="E26">
@@ -1264,23 +1266,23 @@
         <v>5.5917402519469472E-2</v>
       </c>
       <c r="F26">
-        <f>EXP(-lambda)*E26*D26/C26</f>
+        <f t="shared" si="0"/>
         <v>2.4182319083562124E-31</v>
       </c>
       <c r="H26">
-        <f>const^B26*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000018E-17</v>
       </c>
       <c r="I26">
         <f>_xll.BELL($H$11:H26)</f>
-        <v>1.2306878500000023E-12</v>
+        <v>4.847070993100009E-9</v>
       </c>
       <c r="J26">
         <f>_xll.HERMITE(B25, x)</f>
         <v>0</v>
       </c>
       <c r="K26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1289,11 +1291,11 @@
         <v>17</v>
       </c>
       <c r="C27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>355687428096000</v>
       </c>
       <c r="D27">
-        <f>lambda^B27</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000018E-17</v>
       </c>
       <c r="E27">
@@ -1301,24 +1303,24 @@
         <v>4.551397732154977E-2</v>
       </c>
       <c r="F27">
-        <f>EXP(-lambda)*E27*D27/C27</f>
+        <f t="shared" si="0"/>
         <v>1.1578354046593732E-33</v>
       </c>
       <c r="H27">
-        <f>const^B27*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000018E-18</v>
       </c>
       <c r="I27">
         <f>_xll.BELL($H$11:H27)</f>
-        <v>5.2451016000000114E-13</v>
+        <v>2.0675084169600042E-9</v>
       </c>
       <c r="J27">
         <f>_xll.HERMITE(B26, x)</f>
         <v>2027025</v>
       </c>
       <c r="K27">
-        <f t="shared" si="0"/>
-        <v>2.9891278777135916E-21</v>
+        <f t="shared" si="2"/>
+        <v>1.1782511603860318E-17</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1326,11 +1328,11 @@
         <v>18</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6402373705728000</v>
       </c>
       <c r="D28">
-        <f>lambda^B28</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000018E-18</v>
       </c>
       <c r="E28">
@@ -1338,23 +1340,23 @@
         <v>3.6726955698726305E-2</v>
       </c>
       <c r="F28">
-        <f>EXP(-lambda)*E28*D28/C28</f>
+        <f t="shared" si="0"/>
         <v>5.1905629527725153E-36</v>
       </c>
       <c r="H28">
-        <f>const^B28*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000019E-19</v>
       </c>
       <c r="I28">
         <f>_xll.BELL($H$11:H28)</f>
-        <v>2.3446763600000056E-13</v>
+        <v>9.2431427178880142E-10</v>
       </c>
       <c r="J28">
         <f>_xll.HERMITE(B27, x)</f>
         <v>0</v>
       </c>
       <c r="K28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1363,11 +1365,11 @@
         <v>19</v>
       </c>
       <c r="C29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.21645100408832E+17</v>
       </c>
       <c r="D29">
-        <f>lambda^B29</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000019E-19</v>
       </c>
       <c r="E29">
@@ -1375,24 +1377,24 @@
         <v>2.9378980040409397E-2</v>
       </c>
       <c r="F29">
-        <f>EXP(-lambda)*E29*D29/C29</f>
+        <f t="shared" si="0"/>
         <v>2.1853079454044345E-38</v>
       </c>
       <c r="H29">
-        <f>const^B29*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000019E-20</v>
       </c>
       <c r="I29">
         <f>_xll.BELL($H$11:H29)</f>
-        <v>1.0964035578500026E-13</v>
+        <v>4.3211863904739083E-10</v>
       </c>
       <c r="J29">
         <f>_xll.HERMITE(B28, x)</f>
         <v>-34459425</v>
       </c>
       <c r="K29">
-        <f t="shared" si="0"/>
-        <v>-3.1058740585923524E-23</v>
+        <f t="shared" si="2"/>
+        <v>-1.2240986100805185E-19</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1400,11 +1402,11 @@
         <v>20</v>
       </c>
       <c r="C30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.43290200817664E+18</v>
       </c>
       <c r="D30">
-        <f>lambda^B30</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000022E-20</v>
       </c>
       <c r="E30">
@@ -1412,23 +1414,23 @@
         <v>2.3295467750211796E-2</v>
       </c>
       <c r="F30">
-        <f>EXP(-lambda)*E30*D30/C30</f>
+        <f t="shared" si="0"/>
         <v>8.6639785820388228E-41</v>
       </c>
       <c r="H30">
-        <f>const^B30*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000022E-21</v>
       </c>
       <c r="I30">
         <f>_xll.BELL($H$11:H30)</f>
-        <v>5.3507316794500132E-14</v>
+        <v>2.1084503170985544E-10</v>
       </c>
       <c r="J30">
         <f>_xll.HERMITE(B29, x)</f>
         <v>0</v>
       </c>
       <c r="K30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1437,11 +1439,11 @@
         <v>21</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5.109094217170944E+19</v>
       </c>
       <c r="D31">
-        <f>lambda^B31</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000024E-21</v>
       </c>
       <c r="E31">
@@ -1449,24 +1451,24 @@
         <v>1.8308899851658955E-2</v>
       </c>
       <c r="F31">
-        <f>EXP(-lambda)*E31*D31/C31</f>
+        <f t="shared" si="0"/>
         <v>3.242566483345749E-43</v>
       </c>
       <c r="H31">
-        <f>const^B31*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000024E-22</v>
       </c>
       <c r="I31">
         <f>_xll.BELL($H$11:H31)</f>
-        <v>2.7197069490250068E-14</v>
+        <v>1.0716616786821215E-10</v>
       </c>
       <c r="J31">
         <f>_xll.HERMITE(B30, x)</f>
         <v>654729075</v>
       </c>
       <c r="K31">
-        <f t="shared" si="0"/>
-        <v>3.4852972744593954E-25</v>
+        <f t="shared" si="2"/>
+        <v>1.3733316117724988E-21</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.55000000000000004">
@@ -1474,11 +1476,11 @@
         <v>22</v>
       </c>
       <c r="C32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.1240007277776077E+21</v>
       </c>
       <c r="D32">
-        <f>lambda^B32</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000023E-22</v>
       </c>
       <c r="E32">
@@ -1486,23 +1488,23 @@
         <v>1.4262118410668878E-2</v>
       </c>
       <c r="F32">
-        <f>EXP(-lambda)*E32*D32/C32</f>
+        <f t="shared" si="0"/>
         <v>1.1481218899162595E-45</v>
       </c>
       <c r="H32">
-        <f>const^B32*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000023E-23</v>
       </c>
       <c r="I32">
         <f>_xll.BELL($H$11:H32)</f>
-        <v>1.4371009645850042E-14</v>
+        <v>5.6629726312324664E-11</v>
       </c>
       <c r="J32">
         <f>_xll.HERMITE(B31, x)</f>
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1511,11 +1513,11 @@
         <v>23</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.5852016738884978E+22</v>
       </c>
       <c r="D33">
-        <f>lambda^B33</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000025E-23</v>
       </c>
       <c r="E33">
@@ -1523,24 +1525,24 @@
         <v>1.1010658324411393E-2</v>
       </c>
       <c r="F33">
-        <f>EXP(-lambda)*E33*D33/C33</f>
+        <f t="shared" si="0"/>
         <v>3.8538021036289494E-48</v>
       </c>
       <c r="H33">
-        <f>const^B33*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000025E-24</v>
       </c>
       <c r="I33">
         <f>_xll.BELL($H$11:H33)</f>
-        <v>7.8806637271564695E-15</v>
+        <v>3.1055612394312385E-11</v>
       </c>
       <c r="J33">
         <f>_xll.HERMITE(B32, x)</f>
         <v>-13749310575</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
-        <v>-4.191305236114618E-27</v>
+        <f t="shared" si="2"/>
+        <v>-1.6516825910295962E-23</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -1548,11 +1550,11 @@
         <v>24</v>
       </c>
       <c r="C34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6.2044840173323941E+23</v>
       </c>
       <c r="D34">
-        <f>lambda^B34</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000025E-24</v>
       </c>
       <c r="E34">
@@ -1560,23 +1562,23 @@
         <v>8.4241863993456678E-3</v>
       </c>
       <c r="F34">
-        <f>EXP(-lambda)*E34*D34/C34</f>
+        <f t="shared" si="0"/>
         <v>1.2285500372543286E-50</v>
       </c>
       <c r="H34">
-        <f>const^B34*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000026E-25</v>
       </c>
       <c r="I34">
         <f>_xll.BELL($H$11:H34)</f>
-        <v>4.4777793292542559E-15</v>
+        <v>1.7645960183060643E-11</v>
       </c>
       <c r="J34">
         <f>_xll.HERMITE(B33, x)</f>
         <v>0</v>
       </c>
       <c r="K34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1585,11 +1587,11 @@
         <v>25</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.5511210043330986E+25</v>
       </c>
       <c r="D35">
-        <f>lambda^B35</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000026E-25</v>
       </c>
       <c r="E35">
@@ -1597,24 +1599,24 @@
         <v>6.3871547649431704E-3</v>
       </c>
       <c r="F35">
-        <f>EXP(-lambda)*E35*D35/C35</f>
+        <f t="shared" si="0"/>
         <v>3.7259095905235857E-53</v>
       </c>
       <c r="H35">
-        <f>const^B35*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000026E-26</v>
       </c>
       <c r="I35">
         <f>_xll.BELL($H$11:H35)</f>
-        <v>2.6324359894865243E-15</v>
+        <v>1.0373759677620961E-11</v>
       </c>
       <c r="J35">
         <f>_xll.HERMITE(B34, x)</f>
         <v>316234143225</v>
       </c>
       <c r="K35">
-        <f t="shared" si="0"/>
-        <v>5.3668678162722922E-29</v>
+        <f t="shared" si="2"/>
+        <v>2.1149458968773216E-25</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -1622,11 +1624,11 @@
         <v>26</v>
       </c>
       <c r="C36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.0329146112660565E+26</v>
       </c>
       <c r="D36">
-        <f>lambda^B36</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000028E-26</v>
       </c>
       <c r="E36">
@@ -1634,23 +1636,23 @@
         <v>4.7987965971261759E-3</v>
       </c>
       <c r="F36">
-        <f>EXP(-lambda)*E36*D36/C36</f>
+        <f t="shared" si="0"/>
         <v>1.0766731114250595E-55</v>
       </c>
       <c r="H36">
-        <f>const^B36*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000029E-27</v>
       </c>
       <c r="I36">
         <f>_xll.BELL($H$11:H36)</f>
-        <v>1.5990812421093124E-15</v>
+        <v>6.3014982997410149E-12</v>
       </c>
       <c r="J36">
         <f>_xll.HERMITE(B35, x)</f>
         <v>0</v>
       </c>
       <c r="K36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1659,11 +1661,11 @@
         <v>27</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0888869450418352E+28</v>
       </c>
       <c r="D37">
-        <f>lambda^B37</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000027E-27</v>
       </c>
       <c r="E37">
@@ -1671,24 +1673,24 @@
         <v>3.5726009523997515E-3</v>
       </c>
       <c r="F37">
-        <f>EXP(-lambda)*E37*D37/C37</f>
+        <f t="shared" si="0"/>
         <v>2.968740727549095E-58</v>
       </c>
       <c r="H37">
-        <f>const^B37*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000028E-28</v>
       </c>
       <c r="I37">
         <f>_xll.BELL($H$11:H37)</f>
-        <v>1.0024622897747208E-15</v>
+        <v>3.9503853273874616E-12</v>
       </c>
       <c r="J37">
         <f>_xll.HERMITE(B36, x)</f>
         <v>-7905853580625</v>
       </c>
       <c r="K37">
-        <f t="shared" si="0"/>
-        <v>-7.2783681714105964E-31</v>
+        <f t="shared" si="2"/>
+        <v>-2.8681736086178091E-27</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -1696,11 +1698,11 @@
         <v>28</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3.0488834461171384E+29</v>
       </c>
       <c r="D38">
-        <f>lambda^B38</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000031E-28</v>
       </c>
       <c r="E38">
@@ -1708,23 +1710,23 @@
         <v>2.6354020779049692E-3</v>
       </c>
       <c r="F38">
-        <f>EXP(-lambda)*E38*D38/C38</f>
+        <f t="shared" si="0"/>
         <v>7.8212580238022168E-61</v>
       </c>
       <c r="H38">
-        <f>const^B38*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000032E-29</v>
       </c>
       <c r="I38">
         <f>_xll.BELL($H$11:H38)</f>
-        <v>6.4782327123839916E-16</v>
+        <v>2.5528697972844033E-12</v>
       </c>
       <c r="J38">
         <f>_xll.HERMITE(B37, x)</f>
         <v>0</v>
       </c>
       <c r="K38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1733,11 +1735,11 @@
         <v>29</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.8417619937397008E+30</v>
       </c>
       <c r="D39">
-        <f>lambda^B39</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000032E-29</v>
       </c>
       <c r="E39">
@@ -1745,24 +1747,24 @@
         <v>1.9262091321878838E-3</v>
       </c>
       <c r="F39">
-        <f>EXP(-lambda)*E39*D39/C39</f>
+        <f t="shared" si="0"/>
         <v>1.9712203280298875E-63</v>
       </c>
       <c r="H39">
-        <f>const^B39*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000032E-30</v>
       </c>
       <c r="I39">
         <f>_xll.BELL($H$11:H39)</f>
-        <v>4.310985796739312E-16</v>
+        <v>1.6988302541650096E-12</v>
       </c>
       <c r="J39">
         <f>_xll.HERMITE(B38, x)</f>
         <v>213458046676875</v>
       </c>
       <c r="K39">
-        <f t="shared" si="0"/>
-        <v>1.0407593057529389E-32</v>
+        <f t="shared" si="2"/>
+        <v>4.1013203923199581E-29</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.55000000000000004">
@@ -1770,11 +1772,11 @@
         <v>30</v>
       </c>
       <c r="C40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2.6525285981219103E+32</v>
       </c>
       <c r="D40">
-        <f>lambda^B40</f>
+        <f t="shared" si="1"/>
         <v>1.0000000000000031E-30</v>
       </c>
       <c r="E40">
@@ -1782,23 +1784,23 @@
         <v>1.3948872354922481E-3</v>
       </c>
       <c r="F40">
-        <f>EXP(-lambda)*E40*D40/C40</f>
+        <f t="shared" si="0"/>
         <v>4.7582754263527029E-66</v>
       </c>
       <c r="H40">
-        <f>const^B40*lambda</f>
+        <f t="shared" si="5"/>
         <v>1.0000000000000031E-31</v>
       </c>
       <c r="I40">
         <f>_xll.BELL($H$11:H40)</f>
-        <v>2.9512071835115505E-16</v>
+        <v>1.1629839800267366E-12</v>
       </c>
       <c r="J40">
         <f>_xll.HERMITE(B39, x)</f>
         <v>0</v>
       </c>
       <c r="K40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>